<commit_message>
flops document check and report update
</commit_message>
<xml_diff>
--- a/Flops_tracker.xlsx
+++ b/Flops_tracker.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raunaqrai/Documents/DIS/m2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBFFB22-51D6-6248-A2E8-39421CD7D030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2D085-4B19-504A-BF62-4B38BBD9207D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{70B8AF31-6A09-CD4B-90EB-72451BED2422}"/>
+    <workbookView xWindow="1520" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{70B8AF31-6A09-CD4B-90EB-72451BED2422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>number of training steps</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>flops for 520 token generation:</t>
-  </si>
-  <si>
-    <t>amount of runs I can have for testing</t>
-  </si>
-  <si>
-    <t>therefore I have 15 to play with</t>
   </si>
   <si>
     <t>3c - model evaluation</t>
@@ -168,8 +162,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.00000%"/>
-    <numFmt numFmtId="170" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -223,9 +217,9 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -561,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D758DF-4FAB-4646-82FA-DDEEABFBC1D0}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,7 +886,7 @@
         <v>4.2225199999999997E-2</v>
       </c>
       <c r="H32">
-        <v>0.95550000000000002</v>
+        <v>0.96509999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -944,7 +938,7 @@
         <v>4.2212E-2</v>
       </c>
       <c r="H36" s="12">
-        <v>0.78990000000000005</v>
+        <v>0.80989999999999995</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -982,7 +976,7 @@
         <v>4.2225199999999997E-2</v>
       </c>
       <c r="H39" s="12">
-        <v>0.74439999999999995</v>
+        <v>0.73509999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1002,7 +996,7 @@
         <v>4.2225199999999997E-2</v>
       </c>
       <c r="H40" s="12">
-        <v>0.65510000000000002</v>
+        <v>0.65149999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1031,7 +1025,7 @@
         <v>4.22516E-2</v>
       </c>
       <c r="H42" s="12">
-        <v>0.67879999999999996</v>
+        <v>0.6744</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1051,7 +1045,7 @@
         <v>4.22516E-2</v>
       </c>
       <c r="H43" s="12">
-        <v>0.61470000000000002</v>
+        <v>0.61619999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1074,7 +1068,7 @@
         <v>1.0242100000000001E-2</v>
       </c>
       <c r="H45" s="12">
-        <v>0.70879999999999999</v>
+        <v>0.72289999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1140,7 +1134,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D54" s="1">
         <f>11*B59</f>
@@ -1175,18 +1169,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="1">
-        <f>F57/B59</f>
-        <v>4.6844210526316097</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>39</v>
-      </c>
+      <c r="B60" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
flops rejig for better model evaluation
</commit_message>
<xml_diff>
--- a/Flops_tracker.xlsx
+++ b/Flops_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raunaqrai/Documents/DIS/m2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2D085-4B19-504A-BF62-4B38BBD9207D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4BD407-2B05-BB4D-8430-8F5757FFE202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{70B8AF31-6A09-CD4B-90EB-72451BED2422}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>number of training steps</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>3c - model evaluation</t>
+  </si>
+  <si>
+    <t>amount of tests I can have in total</t>
+  </si>
+  <si>
+    <t>52 tests allowed in total</t>
   </si>
 </sst>
 </file>
@@ -555,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D758DF-4FAB-4646-82FA-DDEEABFBC1D0}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1106,7 @@
         <v>0.33283259999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>33</v>
       </c>
@@ -1109,58 +1115,60 @@
         <v>0.66716740000000008</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F51" s="11">
         <f>B24*F50</f>
         <v>6.6716740000000008E+16</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>35</v>
       </c>
       <c r="B53">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="C53" s="6">
-        <v>6.21E+16</v>
+        <v>5.17E+16</v>
       </c>
       <c r="D53" s="6">
         <v>172000000000000</v>
       </c>
       <c r="F53" s="8">
-        <v>0.62246679999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.51900970000000002</v>
+      </c>
+      <c r="H53" s="12">
+        <v>0.29809999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>38</v>
       </c>
       <c r="D54" s="1">
-        <f>11*B59</f>
-        <v>3135000000000000</v>
+        <v>0</v>
       </c>
       <c r="F54" s="2">
         <f>D54/B24</f>
-        <v>3.1350000000000003E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
         <v>36</v>
       </c>
       <c r="F56" s="9">
         <f>F50-F53-F54</f>
-        <v>1.3350600000000087E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.14815770000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F57" s="1">
         <f>F56*B24</f>
-        <v>1335060000000008.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.4815770000000006E+16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -1168,8 +1176,23 @@
         <v>285000000000000</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61" s="1">
+        <f>F57/B59</f>
+        <v>51.985157894736865</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>